<commit_message>
Statement Summary F14 coulm updated
</commit_message>
<xml_diff>
--- a/OldMutual/Output/ExceptionReportMatchStatus.xlsx
+++ b/OldMutual/Output/ExceptionReportMatchStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91888\OneDrive\Documents\UiPath\Old Mutual Final - Ramesh\Old-Mutual-Excel-Automation\OldMutual\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{618D2D68-A533-4C50-9CE8-C5339729853B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{C361DA1B-0B81-4953-B490-2F8CE7514CF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{3B8BAC9F-FCCB-4F98-A5A5-B868A10F3658}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="52" r:id="rId3"/>
+    <pivotCache cacheId="20" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2312,7 +2312,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Guru Teja" refreshedDate="45282.854655555559" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="2" xr:uid="{8ABE4D05-A0F8-4D10-BFF9-2F4CBC63748F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Guru Teja" refreshedDate="45283.599476620373" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="2" xr:uid="{8ABE4D05-A0F8-4D10-BFF9-2F4CBC63748F}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:R100000" sheet="Untraced Bills"/>
   </cacheSource>
@@ -2426,7 +2426,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{043CB6DA-AE6A-4B7F-A180-332C603A0C7C}" name="PivotTable1" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{043CB6DA-AE6A-4B7F-A180-332C603A0C7C}" name="PivotTable1" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="V1:V2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>

</xml_diff>